<commit_message>
changes in mobile view
</commit_message>
<xml_diff>
--- a/database/payments.xlsx
+++ b/database/payments.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -102,6 +102,60 @@
   </si>
   <si>
     <t>2025-08-18T07:00:18.906Z</t>
+  </si>
+  <si>
+    <t>1756651754825</t>
+  </si>
+  <si>
+    <t>1756651364942</t>
+  </si>
+  <si>
+    <t>1755340190541</t>
+  </si>
+  <si>
+    <t>Ravibhawan Ghar</t>
+  </si>
+  <si>
+    <t>2025-08-24</t>
+  </si>
+  <si>
+    <t>Bank Transfer</t>
+  </si>
+  <si>
+    <t>Nabil</t>
+  </si>
+  <si>
+    <t>security_deposit</t>
+  </si>
+  <si>
+    <t>2025-08-31T14:49:14.825Z</t>
+  </si>
+  <si>
+    <t>1756655343517</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>2025-08-31</t>
+  </si>
+  <si>
+    <t>2025-08-31T15:49:03.518Z</t>
+  </si>
+  <si>
+    <t>1756655447320</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>2026-01-15</t>
+  </si>
+  <si>
+    <t>2025-08-31T15:50:47.320Z</t>
   </si>
 </sst>
 </file>
@@ -478,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
@@ -605,6 +659,183 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>50000</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>50000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4">
+        <v>50000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>50000</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5">
+        <v>50000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>50000</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>